<commit_message>
WinCanvas and SourceCanvas updated
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED2DC58-F29C-4F6A-8116-AC949EDBBF9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C08FE-19E5-4D81-AF58-D4DA739147C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="361">
   <si>
     <t>YOU HAVE COMPLETED A LEVEL!</t>
   </si>
@@ -1101,6 +1101,9 @@
   </si>
   <si>
     <t>idHelpTwoRowsInPlace2</t>
+  </si>
+  <si>
+    <t>idFirstRowCongratulation</t>
   </si>
 </sst>
 </file>
@@ -1496,10 +1499,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1984,848 +1987,859 @@
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C112" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B115" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SourceCanvas updates; Ads added
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C08FE-19E5-4D81-AF58-D4DA739147C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63EBAD2-081B-4902-8499-B479D211D695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="364">
   <si>
     <t>YOU HAVE COMPLETED A LEVEL!</t>
   </si>
@@ -1104,6 +1104,15 @@
   </si>
   <si>
     <t>idFirstRowCongratulation</t>
+  </si>
+  <si>
+    <t>idShowAd</t>
+  </si>
+  <si>
+    <t>This button lets you view an ad and earn some RotoCoins!</t>
+  </si>
+  <si>
+    <t>Нажав эту кнопку, Вы посмотрите рекламу и получите немного РотоКойнов!</t>
   </si>
 </sst>
 </file>
@@ -1499,10 +1508,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2073,773 +2082,784 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B116" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Purchasing added; Shop scene added
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63EBAD2-081B-4902-8499-B479D211D695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA82D4DD-442B-4C8A-8BE7-8C745D49D75A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,9 +508,6 @@
     <t>Bears in Karelia are common inhabitants, and people ususally can watch them going out of the woods.</t>
   </si>
   <si>
-    <t>Медведи в лксах Карелии обитают повсеместно, и часто выходят к людям.</t>
-  </si>
-  <si>
     <t>LevelTitle011</t>
   </si>
   <si>
@@ -1113,6 +1110,9 @@
   </si>
   <si>
     <t>Нажав эту кнопку, Вы посмотрите рекламу и получите немного РотоКойнов!</t>
+  </si>
+  <si>
+    <t>Медведи в лесах Карелии обитают повсеместно, и часто выходят к людям.</t>
   </si>
 </sst>
 </file>
@@ -1510,8 +1510,8 @@
   </sheetPr>
   <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1523,18 +1523,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>28</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>30</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>32</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="19" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>36</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>38</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>40</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="23" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>42</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="24" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>44</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="25" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>46</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>48</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="27" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>50</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="28" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>52</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>54</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>56</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>58</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>60</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="33" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>62</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>64</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>66</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>68</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>70</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>72</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>74</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="40" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>76</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>78</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>80</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>82</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>82</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>84</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>86</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>90</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>92</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>94</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>96</v>
@@ -2084,13 +2084,13 @@
     </row>
     <row r="52" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
         <v>113</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>114</v>
@@ -2332,535 +2332,535 @@
         <v>161</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>162</v>
+        <v>363</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="C91" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="C101" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B116" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="C116" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="C117" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PurchasingManager updates; World updates; Puzzle updates
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA82D4DD-442B-4C8A-8BE7-8C745D49D75A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADCE1D7-5F09-43E6-B7C1-6909DAD51521}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="373">
   <si>
     <t>YOU HAVE COMPLETED A LEVEL!</t>
   </si>
@@ -1113,6 +1113,33 @@
   </si>
   <si>
     <t>Медведи в лесах Карелии обитают повсеместно, и часто выходят к людям.</t>
+  </si>
+  <si>
+    <t>id1000_rotocoins</t>
+  </si>
+  <si>
+    <t>id3000_rotocoins</t>
+  </si>
+  <si>
+    <t>id10000_rotocoins</t>
+  </si>
+  <si>
+    <t>10,000 RotoCoins</t>
+  </si>
+  <si>
+    <t>1,000 RotoCoins</t>
+  </si>
+  <si>
+    <t>3,000 RotoCoins</t>
+  </si>
+  <si>
+    <t>10 000 РотоКойнов</t>
+  </si>
+  <si>
+    <t>1 000 РотоКойнов</t>
+  </si>
+  <si>
+    <t>3 000 РотоКойнов</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1190,6 +1217,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1508,10 +1538,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2863,6 +2893,39 @@
         <v>305</v>
       </c>
     </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Shop updates; audio track & sfx updates
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A83F160-BB2A-4EB3-94AC-24B74283F08B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977E02D4-DC6B-4FA1-BAE9-D57B4EECC5E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="385">
   <si>
     <t>YOU HAVE COMPLETED A LEVEL!</t>
   </si>
@@ -1158,6 +1158,24 @@
   </si>
   <si>
     <t>ХОТИТЕ КУПИТЬ {0}\n ЗА {1}?</t>
+  </si>
+  <si>
+    <t>idRestorePurcases</t>
+  </si>
+  <si>
+    <t>You may restore your purchases by tapping this button.</t>
+  </si>
+  <si>
+    <t>idBackToPuzzle</t>
+  </si>
+  <si>
+    <t>This button returns you to the puzzle.</t>
+  </si>
+  <si>
+    <t>Эта кнопка возвращает\nк головоломке.</t>
+  </si>
+  <si>
+    <t>Эта кнопка восстанавливает\nВаши покупки.</t>
   </si>
 </sst>
 </file>
@@ -1556,10 +1574,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C127" sqref="A1:C127"/>
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2966,6 +2984,28 @@
         <v>378</v>
       </c>
     </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
SourceCanvas & WinCanvas updates, prepare for iOS build
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977E02D4-DC6B-4FA1-BAE9-D57B4EECC5E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6DDBC-1263-4060-8FC6-722C77CD4642}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,12 +1145,6 @@
     <t>ОТКРЫЛСЯ ВХОД\nВ СЛЕДУЮЩЕЕ ЦАРСТВО!</t>
   </si>
   <si>
-    <t>НЕДОСТАТОЧНО РОТОКОЙНОВ ДЛЯ МАГИЧЕСКОГО ХОДА.\nХотите купить РотоКойны?</t>
-  </si>
-  <si>
-    <t>INSUFFICIENT ROTOCOINS TO PERFORM AUTOSTEP.\nDo you want to buy some RotoCoins?</t>
-  </si>
-  <si>
     <t>idPurchaseConfirmation</t>
   </si>
   <si>
@@ -1176,6 +1170,12 @@
   </si>
   <si>
     <t>Эта кнопка восстанавливает\nВаши покупки.</t>
+  </si>
+  <si>
+    <t>INSUFFICIENT ROTOCOINS\nDo you want to buy some?</t>
+  </si>
+  <si>
+    <t>НЕДОСТАТОЧНО РОТОКОЙНОВ\nХотите купить?</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1577,7 @@
   <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2962,48 +2962,48 @@
         <v>368</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>371</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Story intro scene added; pre-TestFlight build
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6DDBC-1263-4060-8FC6-722C77CD4642}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3770CC06-3EC7-4AFD-8F64-36DF0C9F24DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="385">
-  <si>
-    <t>YOU HAVE COMPLETED A LEVEL!</t>
-  </si>
-  <si>
-    <t>УРОВЕНЬ ПРОЙДЕН!</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="418">
   <si>
     <t>GALLERY OPENED!</t>
   </si>
@@ -40,15 +34,9 @@
     <t>МОЛОДЕЦ!</t>
   </si>
   <si>
-    <t>A REALM IS REVEALED!</t>
-  </si>
-  <si>
     <t>ОТКРЫЛОСЬ ЦАРСТВО!</t>
   </si>
   <si>
-    <t>A NEW LEVEL BECOMES PLAYABLE!</t>
-  </si>
-  <si>
     <t>YOU HAVE COMPLETED A REALM!</t>
   </si>
   <si>
@@ -64,24 +52,12 @@
     <t>ИГРА ПРОЙДЕНА!</t>
   </si>
   <si>
-    <t>BACK TO LEVEL SELECTION?</t>
-  </si>
-  <si>
-    <t>ОБРАТНО К ВЫБОРУ УРОВНЯ?</t>
-  </si>
-  <si>
     <t>TAP TO CONTINUE</t>
   </si>
   <si>
     <t>ПРОДОЛЖИТЬ</t>
   </si>
   <si>
-    <t>RESTART THE LEVEL?</t>
-  </si>
-  <si>
-    <t>НАЧАТЬ УРОВЕНЬ ЗАНОВО?</t>
-  </si>
-  <si>
     <t>MOVE THE TILE TO ITS PLACE?\nThis'll cost you 1000 RotoCoins!</t>
   </si>
   <si>
@@ -118,54 +94,24 @@
     <t>НАЧАТЬ ИГРУ ЗАНОВО?</t>
   </si>
   <si>
-    <t>Welcome to RotoChips!\nThis mysterious planet Earth\nhides many wonderful places.\nTry to discover all of them!</t>
-  </si>
-  <si>
-    <t>Добро пожаловать в RotoChips!\nНа таинственной планете Земля\nскрыто много очаровательных мест.\nПопробуйте раскрыть их!</t>
-  </si>
-  <si>
-    <t>Tap this icon to\nreturn back to level selection</t>
-  </si>
-  <si>
-    <t>Эта кнопка возвращает\nк выбору уровня</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tap this icon to restart the level.\nWARNING!\nAll your points you've earned in this level\nwill be lost! </t>
-  </si>
-  <si>
-    <t>Эта кнопка\nначинает уровень заново.\nВНИМАНИЕ!\nВсе очки, полученные на этом\nуровне, обнулятся!</t>
-  </si>
-  <si>
     <t>Tap this icon\nto view the original image</t>
   </si>
   <si>
     <t>Эта кнопка позволяет\nпосмотреть на исходное изображение</t>
   </si>
   <si>
-    <t>If you're stuck while solving\nthe puzzle, tap this icon\nto automagically move\none tile to its place.\nThis action costs\n&lt;color=red&gt;1000 RotoCoins&lt;/color&gt;, however.</t>
-  </si>
-  <si>
     <t>Если поставить плитку на место\nслишком сложно, то эта кнопка\nмагически сделает это за Вас.\nОдин магический ход\nстоит &lt;color=red&gt;1000 РотоКойнов&lt;/color&gt;.</t>
   </si>
   <si>
     <t>This satellite stores all the puzzle images\nyou've assembled so far.</t>
   </si>
   <si>
-    <t>В этом спутнике хранятся\nфотографии всех уровней,\nкоторые Вы собрали.</t>
-  </si>
-  <si>
     <t>This puzzle game has been developed\nand brought to you by\n\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;\n\nPhotographs of wild nature\nwere taken by\n\n&lt;color=yellow&gt;DMITRY ARKHIPOV&lt;/color&gt;\n&lt;color=lightblue&gt;http://dmitryarkhipov.com/&lt;/color&gt;\n\n\n\n\n\nThank you for playing!\n</t>
   </si>
   <si>
     <t>Эту игру-головоломку разработал для Вас\n\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;\n\n\nФотограф дикой природы\n\n&lt;color=yellow&gt;ДМИТРИЙ АРХИПОВ&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.com/&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.ru/&lt;/color&gt;\n\n\n\n\n\n\nСпасибо за игру!\n</t>
   </si>
   <si>
-    <t>And here is\none of them...</t>
-  </si>
-  <si>
-    <t>А вот и одно из них...</t>
-  </si>
-  <si>
     <t>This puzzle game\nhas been developed\nand brought to you by\n\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
   </si>
   <si>
@@ -229,9 +175,6 @@
     <t>This is a score of RotoChip points you've earned while solving this very puzzle.</t>
   </si>
   <si>
-    <t>Это очки RotoChips, полученные на этом уровне.</t>
-  </si>
-  <si>
     <t>This is your actual RotoCoins balance.</t>
   </si>
   <si>
@@ -245,9 +188,6 @@
   </si>
   <si>
     <t>So far, you've assembled two images. From now on you're on your own. Enjoy these crazy brain-crunching puzzles!</t>
-  </si>
-  <si>
-    <t>Ну вот, вы собрали уже две фотографии. Теперь настало время действовать самостоятельно. Желаем успеха в мире этих мозгодробительных головоломок!</t>
   </si>
   <si>
     <t>Great!\nThe first tile is in its place!</t>
@@ -1139,9 +1079,6 @@
     <t>idShopQuestion</t>
   </si>
   <si>
-    <t>МОЖНО ИГРАТЬ\nНА СЛЕДУЮЩЕМ УРОВНЕ!</t>
-  </si>
-  <si>
     <t>ОТКРЫЛСЯ ВХОД\nВ СЛЕДУЮЩЕЕ ЦАРСТВО!</t>
   </si>
   <si>
@@ -1176,6 +1113,168 @@
   </si>
   <si>
     <t>НЕДОСТАТОЧНО РОТОКОЙНОВ\nХотите купить?</t>
+  </si>
+  <si>
+    <t>idHelpCupButton</t>
+  </si>
+  <si>
+    <t>This button shows\nyour game achievements.</t>
+  </si>
+  <si>
+    <t>Эта кнопка показывает ваши\nдостижения в игре.</t>
+  </si>
+  <si>
+    <t>idIntro001</t>
+  </si>
+  <si>
+    <t>idIntro002</t>
+  </si>
+  <si>
+    <t>Когда-то жил художник, рисовавший чудесные картины</t>
+  </si>
+  <si>
+    <t>Он писал их не красками, а светом</t>
+  </si>
+  <si>
+    <t>И потому они были волшебными</t>
+  </si>
+  <si>
+    <t>Каждая страна считала честью иметь хотя бы часть картины Художника Света</t>
+  </si>
+  <si>
+    <t>И картины его делились на части и разлетались по всему миру</t>
+  </si>
+  <si>
+    <t>И люди любовались ими</t>
+  </si>
+  <si>
+    <t>Но время не пощадило чудесные картины</t>
+  </si>
+  <si>
+    <t>Лишь ядовитые пятна красок напоминали о том, что было изображено на них</t>
+  </si>
+  <si>
+    <t>Но есть способ восстановить их чудесный вид!</t>
+  </si>
+  <si>
+    <t>Добро пожаловать в RotoChips!\nКартины Художника Света\nскрыты в самых разных уголках\nпланеты Земля.</t>
+  </si>
+  <si>
+    <t>Welcome to RotoChips!\nThis planet Earth\nhides many wonderful masterpieces\nof the Artist of Light.</t>
+  </si>
+  <si>
+    <t>А вот и один из них...</t>
+  </si>
+  <si>
+    <t>idIntro003</t>
+  </si>
+  <si>
+    <t>idIntro004</t>
+  </si>
+  <si>
+    <t>idIntro005</t>
+  </si>
+  <si>
+    <t>idIntro006</t>
+  </si>
+  <si>
+    <t>idIntro007</t>
+  </si>
+  <si>
+    <t>idIntro008</t>
+  </si>
+  <si>
+    <t>idIntro009</t>
+  </si>
+  <si>
+    <t>idIntro010</t>
+  </si>
+  <si>
+    <t>Once there lived an artist who painted miraculous pictures</t>
+  </si>
+  <si>
+    <t>He created them with Light, not with paints</t>
+  </si>
+  <si>
+    <t>And that's why they became miraculous</t>
+  </si>
+  <si>
+    <t>His masterpieces were divided into parts which spreaded all across the world</t>
+  </si>
+  <si>
+    <t>And people admired them</t>
+  </si>
+  <si>
+    <t>Their light faded, so did their colors</t>
+  </si>
+  <si>
+    <t>But there is a way to revive them!</t>
+  </si>
+  <si>
+    <t>YOU HAVE ASSEMBLED THE PUZZLE!</t>
+  </si>
+  <si>
+    <t>ГОЛОВОЛОМКА СОБРАНА!</t>
+  </si>
+  <si>
+    <t>THE REALM IS REVEALED!</t>
+  </si>
+  <si>
+    <t>A NEW PUZZLE BECOMES PLAYABLE!</t>
+  </si>
+  <si>
+    <t>BACK TO PICTURE SELECTION?</t>
+  </si>
+  <si>
+    <t>ОБРАТНО К ВЫБОРУ КАРТИНЫ?</t>
+  </si>
+  <si>
+    <t>RESTART THE PUZZLE?</t>
+  </si>
+  <si>
+    <t>НАЧАТЬ ГОЛОВОЛОМКУ ЗАНОВО?</t>
+  </si>
+  <si>
+    <t>МОЖНО СОБРАТЬ\nСЛЕДУЮЩУЮ КАРТИНКУ!</t>
+  </si>
+  <si>
+    <t>Эта кнопка возвращает\nк выбору картинки</t>
+  </si>
+  <si>
+    <t>Tap this icon to\nreturn back to puzzle selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap this icon to restart the puzzle.\nWARNING!\nAll your points you've earned in this puzzle\nwill be lost! </t>
+  </si>
+  <si>
+    <t>Эта кнопка\nначинает уровень заново.\nВНИМАНИЕ!\nВсе очки, полученные за эту\nголоволомку, обнулятся!</t>
+  </si>
+  <si>
+    <t>If you're stuck while solving\nthe puzzle, tap this icon\nto automagically move\none tile to its place.\nThis action costs\n&lt;color=red&gt;1,000 RotoCoins&lt;/color&gt;, however.</t>
+  </si>
+  <si>
+    <t>В этом спутнике хранятся\nвсе изображения,\nкоторые Вы собрали.</t>
+  </si>
+  <si>
+    <t>Это очки RotoChips, полученные за эту головоломку.</t>
+  </si>
+  <si>
+    <t>Ну вот, вы собрали уже две картины. Теперь настало время действовать самостоятельно. Желаем успеха в мире этих мозгодробительных головоломок!</t>
+  </si>
+  <si>
+    <t>Свет понемногу ушел из них, и они выцвели</t>
+  </si>
+  <si>
+    <t>What was painted on those pictures could be hardly guessed by acid paint spots on them</t>
+  </si>
+  <si>
+    <t>But time knows no mercy, so the miraculous pictures\ndid not last for the eternity</t>
+  </si>
+  <si>
+    <t>Every country considered it an honor to own at least a part of the Artist's pictures</t>
+  </si>
+  <si>
+    <t>And here is one of them...</t>
   </si>
 </sst>
 </file>
@@ -1574,1436 +1673,1557 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="56.5546875" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" customWidth="1"/>
+    <col min="3" max="3" width="71.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>398</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>399</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>372</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>400</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>402</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>379</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>406</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>407</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>409</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>417</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="C129" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C131" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C132" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
         <v>381</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C133" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C134" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C135" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C136" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="C137" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C138" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C139" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C140" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestFlight build with universal language recognition
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3770CC06-3EC7-4AFD-8F64-36DF0C9F24DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C2CD8-87E8-4AB8-B5C7-02D42C4FF4E5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Эту игру-головоломку разработал для Вас\n\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;\n\n\nФотограф дикой природы\n\n&lt;color=yellow&gt;ДМИТРИЙ АРХИПОВ&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.com/&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.ru/&lt;/color&gt;\n\n\n\n\n\n\nСпасибо за игру!\n</t>
   </si>
   <si>
-    <t>This puzzle game\nhas been developed\nand brought to you by\n\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
-  </si>
-  <si>
     <t>Эту игру-головоломку\nразработал для Вас\n\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
   </si>
   <si>
@@ -1275,6 +1272,9 @@
   </si>
   <si>
     <t>And here is one of them...</t>
+  </si>
+  <si>
+    <t>This puzzle game\nhas been developed\nand brought to you by\n\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1676,7 @@
   <dimension ref="A1:C140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1688,29 +1688,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1743,18 +1743,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1765,18 +1765,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1787,18 +1787,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1809,18 +1809,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1886,40 +1886,40 @@
     </row>
     <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
@@ -1930,10 +1930,10 @@
     </row>
     <row r="23" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>26</v>
@@ -1941,18 +1941,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>28</v>
@@ -1963,1267 +1963,1267 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C74" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="C91" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="C101" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="C115" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B116" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="C116" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="C117" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B125" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="B125" s="7" t="s">
-        <v>345</v>
-      </c>
       <c r="C125" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B127" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="C127" s="7" t="s">
         <v>354</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="C128" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B129" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="C129" s="7" t="s">
         <v>359</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C131" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C132" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C133" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C134" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C135" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C136" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C137" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C138" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C139" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C140" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tutorial logic fixes; new logos added; localization improved
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C2CD8-87E8-4AB8-B5C7-02D42C4FF4E5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64337254-D85B-40BF-888A-2C419FA204BC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,15 +112,6 @@
     <t>Эту игру-головоломку разработал для Вас\n\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;\n\n\nФотограф дикой природы\n\n&lt;color=yellow&gt;ДМИТРИЙ АРХИПОВ&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.com/&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.ru/&lt;/color&gt;\n\n\n\n\n\n\nСпасибо за игру!\n</t>
   </si>
   <si>
-    <t>Эту игру-головоломку\nразработал для Вас\n\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
-  </si>
-  <si>
-    <t>Photographs of wild nature\nwere taken by\n\n&lt;color=yellow&gt;DMITRY ARKHIPOV&lt;/color&gt;\n&lt;color=lightblue&gt;http://dmitryarkhipov.com/&lt;/color&gt;</t>
-  </si>
-  <si>
-    <t>Фотограф дикой природы\n\n&lt;color=yellow&gt;ДМИТРИЙ АРХИПОВ&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.com/&lt;/color&gt;</t>
-  </si>
-  <si>
     <t>THANK YOU FOR PLAYING!</t>
   </si>
   <si>
@@ -1274,7 +1265,16 @@
     <t>And here is one of them...</t>
   </si>
   <si>
-    <t>This puzzle game\nhas been developed\nand brought to you by\n\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;</t>
+    <t>This puzzle game\nhas been developed\nand brought to you by\n&lt;color=yellow&gt;IGOR SPIRIDONOV&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;\n\nAdditional\nlogo design\n&lt;color=yellow&gt;ALINA SPIRIDONOVA&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>Эту игру-головоломку\nразработал для Вас\n&lt;color=yellow&gt;ИГОРЬ СПИРИДОНОВ&lt;/color&gt;\n&lt;color=lightblue&gt;https://vk.com/rotochips&lt;/color&gt;\n\nДополнительный\nдизайн логотипа\n&lt;color=yellow&gt;АЛИНА СПИРИДОНОВА&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>Фотограф дикой природы\n&lt;color=yellow&gt;ДМИТРИЙ АРХИПОВ&lt;/color&gt;\n&lt;color=lightblue&gt;http://www.dmitryarkhipov.com/&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>Photographs of wild nature\nwere shot by\n&lt;color=yellow&gt;DMITRY ARKHIPOV&lt;/color&gt;\n&lt;color=lightblue&gt;http://dmitryarkhipov.com/&lt;/color&gt;</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1676,7 @@
   <dimension ref="A1:C140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1688,29 +1688,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1743,18 +1743,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1765,18 +1765,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1787,18 +1787,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1809,18 +1809,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1886,40 +1886,40 @@
     </row>
     <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
@@ -1930,10 +1930,10 @@
     </row>
     <row r="23" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>26</v>
@@ -1941,18 +1941,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>28</v>
@@ -1963,1267 +1963,1267 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B123" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>345</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B125" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>344</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C131" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C132" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C133" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C134" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C135" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C136" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C137" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C138" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C139" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C140" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Story scene added; Finale fixes; UI fixes; localization fixes
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64337254-D85B-40BF-888A-2C419FA204BC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54CF9E6-19BB-4C21-B2E8-F0953CED1F0C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="421">
   <si>
     <t>GALLERY OPENED!</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>Нажав на эту кнопку,\nигру можно запустить заново,\nзаработать кучу очков\nи стать ЧЕМПИОНОМ RotoChips!</t>
-  </si>
-  <si>
-    <t>You can watch\nthe final rolls anytime\nby tapping this button</t>
-  </si>
-  <si>
-    <t>Нажав эту кнопку,\nможно посмотреть финальные титры.</t>
   </si>
   <si>
     <t>The original image has been cut\ninto pieces, which are shuffled\nin random manner.\nTry to re-assemble the image by tapping the yellow buttons!</t>
@@ -1223,9 +1217,6 @@
     <t>НАЧАТЬ ГОЛОВОЛОМКУ ЗАНОВО?</t>
   </si>
   <si>
-    <t>МОЖНО СОБРАТЬ\nСЛЕДУЮЩУЮ КАРТИНКУ!</t>
-  </si>
-  <si>
     <t>Эта кнопка возвращает\nк выбору картинки</t>
   </si>
   <si>
@@ -1275,6 +1266,24 @@
   </si>
   <si>
     <t>Photographs of wild nature\nwere shot by\n&lt;color=yellow&gt;DMITRY ARKHIPOV&lt;/color&gt;\n&lt;color=lightblue&gt;http://dmitryarkhipov.com/&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>idHelpStartVideoButton</t>
+  </si>
+  <si>
+    <t>You can watch the story of the Artist\of Light by tapping this button.</t>
+  </si>
+  <si>
+    <t>Нажав на эту кнопку,\nможно посмотреть историю\nХудожника Света.</t>
+  </si>
+  <si>
+    <t>You can watch the story of the Artist\nof Light or the final rolls\nby tapping this button</t>
+  </si>
+  <si>
+    <t>Нажав эту кнопку,\nможно посмотреть историю\nХудожника Света или\nфинальные титры.</t>
+  </si>
+  <si>
+    <t>МОЖНО СОБРАТЬ\nСЛЕДУЮЩУЮ ГОЛОВОЛОМКУ!</t>
   </si>
 </sst>
 </file>
@@ -1673,10 +1682,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1688,29 +1697,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1721,7 +1730,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1732,10 +1741,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1743,18 +1752,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1765,18 +1774,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1787,18 +1796,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1809,18 +1818,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1831,7 +1840,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1842,7 +1851,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1853,7 +1862,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
@@ -1864,7 +1873,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -1875,7 +1884,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1886,40 +1895,40 @@
     </row>
     <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
@@ -1930,10 +1939,10 @@
     </row>
     <row r="23" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>26</v>
@@ -1941,18 +1950,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>28</v>
@@ -1963,40 +1972,40 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>30</v>
@@ -2007,7 +2016,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
@@ -2018,7 +2027,7 @@
     </row>
     <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>34</v>
@@ -2027,1203 +2036,1214 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>53</v>
+        <v>405</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B75" s="3" t="s">
+    </row>
+    <row r="77" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="B77" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B76" s="1" t="s">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B77" s="1" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B78" s="1" t="s">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B79" s="1" t="s">
+    </row>
+    <row r="81" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B80" s="1" t="s">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="B82" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B81" s="3" t="s">
+    </row>
+    <row r="83" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="1" t="s">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="1" t="s">
+    </row>
+    <row r="85" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B84" s="1" t="s">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B85" s="3" t="s">
+    </row>
+    <row r="87" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="1" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="C88" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="3" t="s">
+    </row>
+    <row r="89" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="B89" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B88" s="1" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="B90" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="C90" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B89" s="3" t="s">
+    </row>
+    <row r="91" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="B91" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B90" s="1" t="s">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B91" s="3" t="s">
+    </row>
+    <row r="93" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B92" s="1" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="B94" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B93" s="3" t="s">
+    </row>
+    <row r="95" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="1" t="s">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="C96" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B95" s="3" t="s">
+    </row>
+    <row r="97" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B96" s="1" t="s">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="B98" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="C98" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B97" s="3" t="s">
+    </row>
+    <row r="99" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="B99" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B98" s="1" t="s">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B99" s="1" t="s">
+    </row>
+    <row r="101" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B100" s="1" t="s">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="B102" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B101" s="3" t="s">
+    </row>
+    <row r="103" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="B103" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B102" s="1" t="s">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="B104" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="C104" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B103" s="3" t="s">
+    </row>
+    <row r="105" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="B105" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B104" s="1" t="s">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="B106" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="C106" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B105" s="3" t="s">
+    </row>
+    <row r="107" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="B107" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="C107" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B106" s="4" t="s">
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="C108" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B107" s="3" t="s">
+    </row>
+    <row r="109" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="C109" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B108" s="4" t="s">
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="C110" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B109" s="3" t="s">
+    </row>
+    <row r="111" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="B111" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B110" s="1" t="s">
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="B112" s="3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="C112" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B111" s="3" t="s">
+    </row>
+    <row r="113" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="B113" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B112" s="1" t="s">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="B114" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="C114" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B113" s="3" t="s">
+    </row>
+    <row r="115" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="B115" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B114" s="1" t="s">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="B116" s="3" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="C116" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B115" s="3" t="s">
+    </row>
+    <row r="117" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="B117" s="5" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="C117" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B116" s="5" t="s">
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="C118" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B117" s="3" t="s">
+    </row>
+    <row r="119" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="B119" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B118" s="1" t="s">
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="B120" s="3" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="C120" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B119" s="3" t="s">
+    </row>
+    <row r="121" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="B121" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B120" s="1" t="s">
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="B122" s="3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="C122" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B121" s="3" t="s">
+    </row>
+    <row r="123" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="B123" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B124" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>343</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B125" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C125" s="1" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>359</v>
+        <v>338</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>351</v>
+        <v>345</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>357</v>
+        <v>347</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B129" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B131" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="C131" t="s">
-        <v>365</v>
+        <v>358</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>386</v>
+        <v>361</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>383</v>
       </c>
       <c r="C132" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>387</v>
+        <v>362</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="C133" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>412</v>
+        <v>375</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>385</v>
       </c>
       <c r="C134" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C135" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C136" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C137" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B135" s="7" t="s">
+      <c r="B138" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C138" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C135" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B136" s="1" t="s">
+      <c r="C139" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C140" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C136" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="C137" t="s">
+      <c r="C141" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C138" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B139" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="C139" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C140" t="s">
-        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Crunched textures & models; release version
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54CF9E6-19BB-4C21-B2E8-F0953CED1F0C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C968BFB-3A40-415B-9E65-F1F9F654B68A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,9 +1271,6 @@
     <t>idHelpStartVideoButton</t>
   </si>
   <si>
-    <t>You can watch the story of the Artist\of Light by tapping this button.</t>
-  </si>
-  <si>
     <t>Нажав на эту кнопку,\nможно посмотреть историю\nХудожника Света.</t>
   </si>
   <si>
@@ -1284,6 +1281,9 @@
   </si>
   <si>
     <t>МОЖНО СОБРАТЬ\nСЛЕДУЮЩУЮ ГОЛОВОЛОМКУ!</t>
+  </si>
+  <si>
+    <t>You can watch the story of the Artist\nof Light by tapping this button.</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1684,8 @@
   </sheetPr>
   <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1758,7 +1758,7 @@
         <v>393</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2041,21 +2041,21 @@
         <v>312</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>415</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Stress image generation eliminated; WinImageMover bug fixed; localization fixed
</commit_message>
<xml_diff>
--- a/localization/RotoChips Localization.xlsx
+++ b/localization/RotoChips Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\__GITREPO__\RotoChipsEvolution\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C968BFB-3A40-415B-9E65-F1F9F654B68A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9841C8D4-CC3B-42EE-AF09-0C54BB9C438F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,9 +1094,6 @@
     <t>INSUFFICIENT ROTOCOINS\nDo you want to buy some?</t>
   </si>
   <si>
-    <t>НЕДОСТАТОЧНО РОТОКОЙНОВ\nХотите купить?</t>
-  </si>
-  <si>
     <t>idHelpCupButton</t>
   </si>
   <si>
@@ -1284,6 +1281,9 @@
   </si>
   <si>
     <t>You can watch the story of the Artist\nof Light by tapping this button.</t>
+  </si>
+  <si>
+    <t>МАЛО РОТОКОЙНОВ\nХотите купить?</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1684,8 @@
   </sheetPr>
   <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1711,10 +1711,10 @@
         <v>282</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>285</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -1755,10 +1755,10 @@
         <v>286</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1799,10 +1799,10 @@
         <v>290</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1821,10 +1821,10 @@
         <v>297</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
@@ -1898,10 +1898,10 @@
         <v>299</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1909,10 +1909,10 @@
         <v>300</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
@@ -1920,10 +1920,10 @@
         <v>301</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
         <v>303</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>26</v>
@@ -1956,7 +1956,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="66" x14ac:dyDescent="0.25">
@@ -1975,10 +1975,10 @@
         <v>306</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="66" x14ac:dyDescent="0.25">
@@ -1986,10 +1986,10 @@
         <v>307</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
@@ -1997,10 +1997,10 @@
         <v>308</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2041,21 +2041,21 @@
         <v>312</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>44</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,7 +3089,7 @@
         <v>356</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>357</v>
+        <v>420</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3127,123 +3127,123 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C132" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C133" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C134" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C135" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C136" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C137" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C138" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C139" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C140" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C141" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>